<commit_message>
Add test results for ptrace functions
</commit_message>
<xml_diff>
--- a/criu_ptrace.xlsx
+++ b/criu_ptrace.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="189">
   <si>
     <t xml:space="preserve">功能</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">test/zdtm/static/seccomp_filter_tsync.c:93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test/zdtm/static/seccomp_filter.c:142</t>
   </si>
   <si>
     <t xml:space="preserve">test/zdtm/static/seccomp_filter_threads.c:90</t>
@@ -69,8 +72,141 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">PTRACE_PEEKUSER (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">仅 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">x86)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:424</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_PEEKUSER, pid, offsetof(user_regs_struct64, cs), 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRACE_POKEDATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/ptrace.c:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_POKEDATA, pid, a + w, s[w])</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PTRACE_POKEUSER (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">仅 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">x86)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_POKEUSER, pid, offsetof(struct user, u_debugreg[DR_FIRSTADDR]), addr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_POKEUSER, pid, offsetof(struct user, u_debugreg[DR_CONTROL]), X86_DR_LOCAL_ENABLE(DR_FIRSTADDR))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:529</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_POKEUSER, pid, offsetof(struct user, u_debugreg[DR_CONTROL]), 0)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PTRACE_GETFPREGS (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">仅 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ppc64 x86)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/arch/ppc64/src/lib/infect.c:206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_GETFPREGS, pid, 0, (void *)&amp;fp-&gt;fpregs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_GETFPREGS, pid, NULL, xsave)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PTRACE_GETVRREGS (</t>
     </r>
     <r>
       <rPr>
@@ -85,24 +221,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">x86)</t>
+      <t xml:space="preserve">ppc64)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:424</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ptrace(PTRACE_PEEKUSER, pid, offsetof(user_regs_struct64, cs), 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTRACE_POKEDATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compel/src/lib/ptrace.c:57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ptrace(PTRACE_POKEDATA, pid, a + w, s[w])</t>
+    <t xml:space="preserve">compel/arch/ppc64/src/lib/infect.c:217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_GETVRREGS, pid, 0, (void*)&amp;fp-&gt;vrregs)</t>
   </si>
   <si>
     <r>
@@ -110,8 +238,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">PTRACE_POKEUSER (</t>
+      <t xml:space="preserve">PTRACE_GETVSRREGS (</t>
     </r>
     <r>
       <rPr>
@@ -126,27 +255,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">x86)</t>
+      <t xml:space="preserve">ppc64)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:502</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ptrace(PTRACE_POKEUSER, pid, offsetof(struct user, u_debugreg[DR_FIRSTADDR]), addr)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:510</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ptrace(PTRACE_POKEUSER, pid, offsetof(struct user, u_debugreg[DR_CONTROL]), X86_DR_LOCAL_ENABLE(DR_FIRSTADDR))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:529</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ptrace(PTRACE_POKEUSER, pid, offsetof(struct user, u_debugreg[DR_CONTROL]), 0)</t>
+    <t xml:space="preserve">compel/arch/ppc64/src/lib/infect.c:244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_GETVSRREGS, pid, 0, (void*)fp-&gt;vsxregs)</t>
   </si>
   <si>
     <r>
@@ -154,8 +272,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">PTRACE_GETFPREGS (</t>
+      <t xml:space="preserve">PTRACE_GETVFPREGS (</t>
     </r>
     <r>
       <rPr>
@@ -170,26 +289,33 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">ppc64 x86)</t>
+      <t xml:space="preserve">arm)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">compel/arch/ppc64/src/lib/infect.c:206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ptrace(PTRACE_GETFPREGS, pid, 0, (void *)&amp;fp-&gt;fpregs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compel/arch/x86/src/lib/infect.c:252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ptrace(PTRACE_GETFPREGS, pid, NULL, xsave)</t>
+    <t xml:space="preserve">compel/arch/arm/src/lib/infect.c:77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_GETVFPREGS, pid, NULL, &amp;vfp)</t>
   </si>
   <si>
     <t xml:space="preserve">PTRACE_GETREGSET</t>
   </si>
   <si>
+    <t xml:space="preserve">criu/arch/s390/crtools.c:623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_GETREGSET, pid, NT_PRSTATUS, &amp;iov)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/arch/x86/kerndat.c:241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_GETREGSET, child, (unsigned)NT_X86_XSTATE, &amp;iov)</t>
+  </si>
+  <si>
     <t xml:space="preserve">test/zdtm/static/s390x_regs_check.c:375</t>
   </si>
   <si>
@@ -229,9 +355,6 @@
     <t xml:space="preserve">compel/arch/s390/src/lib/infect.c:287</t>
   </si>
   <si>
-    <t xml:space="preserve">ptrace(PTRACE_GETREGSET, pid, NT_PRSTATUS, &amp;iov)</t>
-  </si>
-  <si>
     <t xml:space="preserve">compel/arch/s390/src/lib/infect.c:326</t>
   </si>
   <si>
@@ -274,6 +397,18 @@
     <t xml:space="preserve">PTRACE_SETREGSET</t>
   </si>
   <si>
+    <t xml:space="preserve">criu/arch/s390/crtools.c:531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SETREGSET, pid, set, iov)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/arch/s390/crtools.c:630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SETREGSET, pid, NT_PRSTATUS, &amp;iov)</t>
+  </si>
+  <si>
     <t xml:space="preserve">test/zdtm/static/s390x_regs_check.c:319</t>
   </si>
   <si>
@@ -283,9 +418,6 @@
     <t xml:space="preserve">compel/arch/s390/src/lib/infect.c:308</t>
   </si>
   <si>
-    <t xml:space="preserve">ptrace(PTRACE_SETREGSET, pid, NT_PRSTATUS, &amp;iov)</t>
-  </si>
-  <si>
     <t xml:space="preserve">compel/arch/s390/src/lib/infect.c:703</t>
   </si>
   <si>
@@ -412,7 +544,7 @@
     <t xml:space="preserve">ptrace(PTRACE_CONT, stopped, (char *)1, NULL)</t>
   </si>
   <si>
-    <t xml:space="preserve">test/zdtm/static/ptrace_sig.c</t>
+    <t xml:space="preserve">test/zdtm/static/ptrace_sig.c:136</t>
   </si>
   <si>
     <t xml:space="preserve">ptrace(PTRACE_CONT, pid, 0, WSTOPSIG(status)</t>
@@ -437,6 +569,177 @@
   </si>
   <si>
     <t xml:space="preserve">parasite_run(pid, PTRACE_CONT, ctl-&gt;ictx.syscall_ip, 0, regs, &amp;ctl-&gt;orig)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:583</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parasite_run(ctl-&gt;rpid, PTRACE_CONT, ip, 0, &amp;regs, &amp;ctl-&gt;orig)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parasite_run(pid, PTRACE_CONT, ctl-&gt;parasite_ip, ctl-&gt;rstack, &amp;regs, &amp;ctl-&gt;orig)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:1364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parasite_run(pid, PTRACE_CONT, ctl-&gt;parasite_ip, stack, &amp;regs, octx)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRACE_SYSCALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:1387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parasite_run(pid, PTRACE_SYSCALL, addr, ctl-&gt;rstack, &amp;regs, &amp;ctl-&gt;orig)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:1425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SYSCALL, pid, NULL, NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:1517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:1537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRACE_INTERRUPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/seize.c:125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_INTERRUPT, pid, NULL, NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/cr-restore.c:1819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_INTERRUPT, pid, 0, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/cr-restore.c:1870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:1218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRACE_ATTACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/cr-check.c:574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_ATTACH, pid, NULL, NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test/zdtm/transition/ptrace.c:76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_ATTACH, pids[i], (char *)1, NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test/zdtm/static/s390x_regs_check.c:471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_ATTACH, pid, 0, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRACE_SEIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/cr-restore.c:1814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SEIZE, pid, 0, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/cr-restore.c:2095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SEIZE, init-&gt;pid-&gt;real, 0, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SEIZE, pid, NULL, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRACE_SECCOMP_GET_FILTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/seccomp.c:144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SECCOMP_GET_FILTER, entry-&gt;tid_real, i, buf)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/cr-check.c:666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SECCOMP_GET_FILTER, pid, 0, NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRACE_SECCOMP_GET_METADATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/seccomp.c:158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_SECCOMP_GET_METADATA, entry-&gt;tid_real, sizeof(*meta), meta)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRACE_DETACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/seize.c:240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_DETACH, pid, NULL, NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/seize.c:544</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_DETACH, item-&gt;threads[i].real, NULL, NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criu/cr-restore.c:1954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_DETACH, pid, NULL, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test/zdtm/transition/ptrace.c:110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_DETACH, stopped, (char *)1, NULL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test/zdtm/static/s390x_regs_check.c:487</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptrace(PTRACE_DETACH, pid, 0, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compel/src/lib/infect.c:342</t>
   </si>
 </sst>
 </file>
@@ -446,11 +749,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -466,6 +770,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -540,51 +850,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{D3116B15-D1A1-4777-9D21-D37A8C61B798}">
-  <header guid="{D3116B15-D1A1-4777-9D21-D37A8C61B798}" dateTime="2019-08-30T17:36:00.000000000Z" userName="Wenbin Lv" r:id="rId1" minRId="1" maxRId="1" maxSheetId="2">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-</headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="1" ua="false" sId="1">
-    <nc r="C57" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">parasite_run(pid, PTRACE_CONT, ctl-&gt;ictx.syscall_ip, 0, regs, &amp;ctl-&gt;orig)</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.18"/>
@@ -646,104 +923,107 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="B11" s="0" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="B14" s="0" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="C15" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="B16" s="0" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>37</v>
       </c>
@@ -752,204 +1032,204 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="B18" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="B19" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="B31" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="0" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="B41" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,111 +1241,111 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="B43" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="C43" s="0" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="0" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="B49" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="C49" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="0" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+      <c r="C50" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B51" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C51" s="0" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="B53" s="0" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+      <c r="C53" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,23 +1357,343 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>112</v>
+      </c>
       <c r="B56" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="2"/>
+      <c r="A58" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>177</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>